<commit_message>
Log 4j and other work
</commit_message>
<xml_diff>
--- a/VP5_Cucumber_TestNG/TestData/Routing _no.xlsx
+++ b/VP5_Cucumber_TestNG/TestData/Routing _no.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="108">
   <si>
     <t>BankMasterId</t>
   </si>
@@ -343,9 +343,6 @@
   </si>
   <si>
     <t>345345345</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>Status</t>
@@ -680,7 +677,7 @@
   <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -720,9 +717,6 @@
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
-        <v>107</v>
-      </c>
       <c r="D2" s="3">
         <v>67999</v>
       </c>
@@ -743,9 +737,6 @@
       <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
       <c r="D3" s="3">
         <v>68589</v>
       </c>
@@ -766,9 +757,6 @@
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B4" t="s">
-        <v>107</v>
-      </c>
       <c r="D4">
         <v>69254</v>
       </c>
@@ -789,9 +777,6 @@
       <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
       <c r="D5">
         <v>69464</v>
       </c>
@@ -812,9 +797,6 @@
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B6" t="s">
-        <v>107</v>
-      </c>
       <c r="D6">
         <v>69974</v>
       </c>
@@ -835,9 +817,6 @@
       <c r="A7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
-        <v>107</v>
-      </c>
       <c r="D7">
         <v>70628</v>
       </c>
@@ -858,9 +837,6 @@
       <c r="A8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B8" t="s">
-        <v>107</v>
-      </c>
       <c r="D8">
         <v>71450</v>
       </c>
@@ -881,9 +857,6 @@
       <c r="A9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B9" t="s">
-        <v>107</v>
-      </c>
       <c r="D9">
         <v>72284</v>
       </c>
@@ -904,9 +877,6 @@
       <c r="A10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B10" t="s">
-        <v>107</v>
-      </c>
       <c r="D10">
         <v>72917</v>
       </c>
@@ -927,9 +897,6 @@
       <c r="A11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
       <c r="D11">
         <v>77372</v>
       </c>
@@ -950,9 +917,6 @@
       <c r="A12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B12" t="s">
-        <v>107</v>
-      </c>
       <c r="D12">
         <v>77374</v>
       </c>
@@ -973,9 +937,6 @@
       <c r="A13" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B13" t="s">
-        <v>107</v>
-      </c>
       <c r="D13">
         <v>78833</v>
       </c>
@@ -996,9 +957,6 @@
       <c r="A14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
-        <v>107</v>
-      </c>
       <c r="D14">
         <v>79267</v>
       </c>
@@ -1019,9 +977,6 @@
       <c r="A15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B15" t="s">
-        <v>107</v>
-      </c>
       <c r="D15">
         <v>79410</v>
       </c>
@@ -1042,9 +997,6 @@
       <c r="A16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B16" t="s">
-        <v>107</v>
-      </c>
       <c r="D16">
         <v>80493</v>
       </c>
@@ -1065,9 +1017,6 @@
       <c r="A17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B17" t="s">
-        <v>107</v>
-      </c>
       <c r="D17">
         <v>82309</v>
       </c>
@@ -1088,9 +1037,6 @@
       <c r="A18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B18" t="s">
-        <v>107</v>
-      </c>
       <c r="D18">
         <v>83732</v>
       </c>
@@ -1111,9 +1057,6 @@
       <c r="A19" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B19" t="s">
-        <v>107</v>
-      </c>
       <c r="D19">
         <v>83918</v>
       </c>
@@ -1134,9 +1077,6 @@
       <c r="A20" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B20" t="s">
-        <v>107</v>
-      </c>
       <c r="D20">
         <v>84094</v>
       </c>
@@ -1157,9 +1097,6 @@
       <c r="A21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B21" t="s">
-        <v>107</v>
-      </c>
       <c r="D21">
         <v>84513</v>
       </c>
@@ -1180,9 +1117,6 @@
       <c r="A22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B22" t="s">
-        <v>107</v>
-      </c>
       <c r="D22">
         <v>85509</v>
       </c>
@@ -1203,9 +1137,6 @@
       <c r="A23" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
-        <v>107</v>
-      </c>
       <c r="D23">
         <v>86264</v>
       </c>
@@ -1226,9 +1157,6 @@
       <c r="A24" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B24" t="s">
-        <v>107</v>
-      </c>
       <c r="D24">
         <v>86380</v>
       </c>
@@ -1249,9 +1177,6 @@
       <c r="A25" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B25" t="s">
-        <v>107</v>
-      </c>
       <c r="D25">
         <v>86623</v>
       </c>
@@ -1272,9 +1197,6 @@
       <c r="A26" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B26" t="s">
-        <v>107</v>
-      </c>
       <c r="D26">
         <v>87076</v>
       </c>
@@ -1295,9 +1217,6 @@
       <c r="A27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B27" t="s">
-        <v>107</v>
-      </c>
       <c r="D27">
         <v>87078</v>
       </c>
@@ -1318,9 +1237,6 @@
       <c r="A28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B28" t="s">
-        <v>107</v>
-      </c>
       <c r="D28">
         <v>87090</v>
       </c>
@@ -1341,9 +1257,6 @@
       <c r="A29" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B29" t="s">
-        <v>107</v>
-      </c>
       <c r="D29">
         <v>87095</v>
       </c>
@@ -1364,9 +1277,6 @@
       <c r="A30" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B30" t="s">
-        <v>107</v>
-      </c>
       <c r="D30">
         <v>87130</v>
       </c>
@@ -1387,9 +1297,6 @@
       <c r="A31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B31" t="s">
-        <v>107</v>
-      </c>
       <c r="D31">
         <v>87133</v>
       </c>
@@ -1410,9 +1317,6 @@
       <c r="A32" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B32" t="s">
-        <v>107</v>
-      </c>
       <c r="D32">
         <v>87177</v>
       </c>
@@ -1433,9 +1337,6 @@
       <c r="A33" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B33" t="s">
-        <v>107</v>
-      </c>
       <c r="D33">
         <v>87546</v>
       </c>
@@ -1456,9 +1357,6 @@
       <c r="A34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B34" t="s">
-        <v>107</v>
-      </c>
       <c r="D34">
         <v>90582</v>
       </c>
@@ -1479,9 +1377,6 @@
       <c r="A35" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B35" t="s">
-        <v>107</v>
-      </c>
       <c r="D35">
         <v>90618</v>
       </c>
@@ -1502,9 +1397,6 @@
       <c r="A36" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B36" t="s">
-        <v>107</v>
-      </c>
       <c r="D36">
         <v>91004</v>
       </c>
@@ -1525,9 +1417,6 @@
       <c r="A37" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B37" t="s">
-        <v>107</v>
-      </c>
       <c r="D37">
         <v>91028</v>
       </c>
@@ -1548,9 +1437,6 @@
       <c r="A38" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B38" t="s">
-        <v>107</v>
-      </c>
       <c r="D38">
         <v>91465</v>
       </c>
@@ -1571,9 +1457,6 @@
       <c r="A39" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B39" t="s">
-        <v>107</v>
-      </c>
       <c r="D39">
         <v>91725</v>
       </c>
@@ -1594,9 +1477,6 @@
       <c r="A40" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B40" t="s">
-        <v>107</v>
-      </c>
       <c r="D40">
         <v>92129</v>
       </c>
@@ -1617,9 +1497,6 @@
       <c r="A41" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B41" t="s">
-        <v>107</v>
-      </c>
       <c r="D41">
         <v>92243</v>
       </c>
@@ -1640,9 +1517,6 @@
       <c r="A42" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B42" t="s">
-        <v>107</v>
-      </c>
       <c r="D42">
         <v>92293</v>
       </c>
@@ -1663,9 +1537,6 @@
       <c r="A43" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B43" t="s">
-        <v>107</v>
-      </c>
       <c r="D43">
         <v>92312</v>
       </c>
@@ -1686,9 +1557,6 @@
       <c r="A44" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B44" t="s">
-        <v>107</v>
-      </c>
       <c r="D44">
         <v>92330</v>
       </c>
@@ -1709,9 +1577,6 @@
       <c r="A45" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B45" t="s">
-        <v>107</v>
-      </c>
       <c r="D45">
         <v>92363</v>
       </c>
@@ -1732,9 +1597,6 @@
       <c r="A46" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B46" t="s">
-        <v>107</v>
-      </c>
       <c r="D46">
         <v>92423</v>
       </c>
@@ -1755,9 +1617,6 @@
       <c r="A47" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B47" t="s">
-        <v>107</v>
-      </c>
       <c r="D47">
         <v>92444</v>
       </c>
@@ -1778,9 +1637,6 @@
       <c r="A48" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B48" t="s">
-        <v>107</v>
-      </c>
       <c r="D48">
         <v>92448</v>
       </c>
@@ -1801,9 +1657,6 @@
       <c r="A49" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B49" t="s">
-        <v>107</v>
-      </c>
       <c r="D49">
         <v>92450</v>
       </c>
@@ -1824,9 +1677,6 @@
       <c r="A50" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B50" t="s">
-        <v>107</v>
-      </c>
       <c r="D50">
         <v>92514</v>
       </c>
@@ -1847,9 +1697,6 @@
       <c r="A51" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B51" t="s">
-        <v>107</v>
-      </c>
       <c r="D51">
         <v>92518</v>
       </c>
@@ -1870,9 +1717,6 @@
       <c r="A52" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B52" t="s">
-        <v>107</v>
-      </c>
       <c r="D52">
         <v>92545</v>
       </c>
@@ -1892,9 +1736,6 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B53" t="s">
-        <v>107</v>
       </c>
       <c r="D53">
         <v>92572</v>

</xml_diff>